<commit_message>
i added dates to my tasks
i added dates to my tasks and i will be making changes on this file during this month
</commit_message>
<xml_diff>
--- a/PFF-202/Stagiaires/Ramzi Ismail.xlsx
+++ b/PFF-202/Stagiaires/Ramzi Ismail.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="12240" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>Tâche</t>
   </si>
@@ -101,6 +101,9 @@
   </si>
   <si>
     <t>Date Fin</t>
+  </si>
+  <si>
+    <t>/</t>
   </si>
 </sst>
 </file>
@@ -245,7 +248,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -280,7 +283,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -492,17 +495,17 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="23.75" customWidth="1"/>
-    <col min="3" max="3" width="17.125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="26.375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="11.625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.42578125" style="2" customWidth="1"/>
+    <col min="6" max="6" width="11.5703125" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -545,7 +548,7 @@
         <v>42805</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -565,7 +568,7 @@
         <v>42807</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>26</v>
       </c>
@@ -585,7 +588,7 @@
         <v>42810</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>26</v>
       </c>
@@ -618,6 +621,12 @@
       <c r="D6" s="1" t="s">
         <v>22</v>
       </c>
+      <c r="E6" s="3">
+        <v>42813</v>
+      </c>
+      <c r="F6" s="3">
+        <v>42813</v>
+      </c>
     </row>
     <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -632,6 +641,12 @@
       <c r="D7" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="E7" s="3">
+        <v>42814</v>
+      </c>
+      <c r="F7" s="3">
+        <v>42815</v>
+      </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -646,6 +661,12 @@
       <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="E8" s="3">
+        <v>42814</v>
+      </c>
+      <c r="F8" s="3">
+        <v>42824</v>
+      </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
@@ -654,8 +675,14 @@
       <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E9" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
@@ -665,8 +692,14 @@
       <c r="C10" s="1" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="E10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>26</v>
       </c>
@@ -676,8 +709,14 @@
       <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+      <c r="E11" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="75" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>13</v>
       </c>
@@ -686,6 +725,12 @@
       </c>
       <c r="D12" s="1" t="s">
         <v>25</v>
+      </c>
+      <c r="E12" s="3">
+        <v>42850</v>
+      </c>
+      <c r="F12" s="3">
+        <v>42855</v>
       </c>
     </row>
   </sheetData>

</xml_diff>